<commit_message>
Added the updated version of Supplemental Table 6.
</commit_message>
<xml_diff>
--- a/Analysis/Genomics_manuscript_TIR/Supplemental_Figures/Supplemental_Table_6.xlsx
+++ b/Analysis/Genomics_manuscript_TIR/Supplemental_Figures/Supplemental_Table_6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work_Files\GCMP_TIR\immunity_microbiome\Supplemental_Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF811E4-A2AB-4085-B720-9E9161FFA5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B60042-BCC7-450C-9CAA-9294BDAAEE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3132" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{0DB15E06-3AC2-41F8-A19D-0B30620B5E91}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DB15E06-3AC2-41F8-A19D-0B30620B5E91}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S6" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
-    <t>Trait table of genomic and microbiome traits of coral species analyzed in the study.</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
@@ -206,7 +203,10 @@
     <t>POR_Porites_rus</t>
   </si>
   <si>
-    <t>Table S6</t>
+    <t>Table S6: Trait table of genomic and microbiome traits of coral species analyzed in the study</t>
+  </si>
+  <si>
+    <t>Trait table of genomic and microbiome traits of coral species used to conducted the analysis in this study. Immune families were annotated using available genomes and HMMER. Microbiome data was optained from the GCMP data set and analyzed by compartment (all, mucus, tissue, and skeleton) in QIIME2.</t>
   </si>
 </sst>
 </file>
@@ -282,14 +282,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,7 +607,7 @@
   <dimension ref="A1:AM14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -654,1453 +654,1479 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:39" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="T3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="U3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="V3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="W3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="X3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="Y3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Z3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Z3" s="4" t="s">
+      <c r="AA3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AB3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AC3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AC3" s="4" t="s">
+      <c r="AD3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AD3" s="4" t="s">
+      <c r="AE3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AE3" s="4" t="s">
+      <c r="AF3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AF3" s="4" t="s">
+      <c r="AG3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AH3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AI3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AK3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AK3" s="4" t="s">
+      <c r="AL3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AL3" s="4" t="s">
+      <c r="AM3" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="AM3" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>38</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>37</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>16</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>11</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>1299</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="3">
         <v>426</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="3">
         <v>8</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="3">
         <v>1902</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="3">
         <v>495</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="3">
         <v>44.157894740000003</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="3">
         <v>3.7879999999999998</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="3">
         <v>0.13472216000000001</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="3">
         <v>0.98045260000000001</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q4" s="3">
         <v>0.2187038</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="3">
         <v>21.1351376</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4" s="3">
         <v>16</v>
       </c>
-      <c r="T4" s="5">
+      <c r="T4" s="3">
         <v>50.25</v>
       </c>
-      <c r="U4" s="5">
+      <c r="U4" s="3">
         <v>3.9170105469999998</v>
       </c>
-      <c r="V4" s="5">
+      <c r="V4" s="3">
         <v>0.11341809999999999</v>
       </c>
-      <c r="W4" s="5">
+      <c r="W4" s="3">
         <v>0.95429019999999998</v>
       </c>
-      <c r="X4" s="5">
+      <c r="X4" s="3">
         <v>0.20921466999999999</v>
       </c>
-      <c r="Y4" s="5">
+      <c r="Y4" s="3">
         <v>23.906673000000001</v>
       </c>
-      <c r="Z4" s="5">
+      <c r="Z4" s="3">
         <v>10</v>
       </c>
-      <c r="AA4" s="5">
+      <c r="AA4" s="3">
         <v>30.6</v>
       </c>
-      <c r="AB4" s="5">
+      <c r="AB4" s="3">
         <v>3.4210000090000001</v>
       </c>
-      <c r="AC4" s="5">
+      <c r="AC4" s="3">
         <v>0.1589334</v>
       </c>
-      <c r="AD4" s="5">
+      <c r="AD4" s="3">
         <v>0.93784559999999995</v>
       </c>
-      <c r="AE4" s="5">
+      <c r="AE4" s="3">
         <v>0.22906199999999999</v>
       </c>
-      <c r="AF4" s="5">
+      <c r="AF4" s="3">
         <v>14.524756699999999</v>
       </c>
-      <c r="AG4" s="5">
+      <c r="AG4" s="3">
         <v>12</v>
       </c>
-      <c r="AH4" s="5">
+      <c r="AH4" s="3">
         <v>42.083333000000003</v>
       </c>
-      <c r="AI4" s="5">
+      <c r="AI4" s="3">
         <v>3.7396517720000002</v>
       </c>
-      <c r="AJ4" s="5">
+      <c r="AJ4" s="3">
         <v>0.1406558</v>
       </c>
-      <c r="AK4" s="5">
+      <c r="AK4" s="3">
         <v>0.95579400000000003</v>
       </c>
-      <c r="AL4" s="5">
+      <c r="AL4" s="3">
         <v>0.2419095</v>
       </c>
-      <c r="AM4" s="5">
+      <c r="AM4" s="3">
         <v>20.884041</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>33</v>
+      </c>
+      <c r="F5" s="3">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1308</v>
+      </c>
+      <c r="I5" s="3">
+        <v>528</v>
+      </c>
+      <c r="J5" s="3">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1903</v>
+      </c>
+      <c r="L5" s="3">
+        <v>548</v>
+      </c>
+      <c r="M5" s="3">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="N5" s="3">
+        <v>3.6190000000000002</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.2303354</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0.9572117</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.175399</v>
+      </c>
+      <c r="R5" s="3">
+        <v>20.853458</v>
+      </c>
+      <c r="S5" s="3">
+        <v>2</v>
+      </c>
+      <c r="T5" s="3">
         <v>42</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="5">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5">
-        <v>33</v>
-      </c>
-      <c r="F5" s="5">
-        <v>17</v>
-      </c>
-      <c r="G5" s="5">
-        <v>10</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1308</v>
-      </c>
-      <c r="I5" s="5">
-        <v>528</v>
-      </c>
-      <c r="J5" s="5">
-        <v>7</v>
-      </c>
-      <c r="K5" s="5">
-        <v>1903</v>
-      </c>
-      <c r="L5" s="5">
-        <v>548</v>
-      </c>
-      <c r="M5" s="5">
-        <v>37.299999999999997</v>
-      </c>
-      <c r="N5" s="5">
-        <v>3.6190000000000002</v>
-      </c>
-      <c r="O5" s="5">
-        <v>0.2303354</v>
-      </c>
-      <c r="P5" s="5">
-        <v>0.9572117</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>0.175399</v>
-      </c>
-      <c r="R5" s="5">
-        <v>20.853458</v>
-      </c>
-      <c r="S5" s="5">
-        <v>2</v>
-      </c>
-      <c r="T5" s="5">
-        <v>42</v>
-      </c>
-      <c r="U5" s="5">
+      <c r="U5" s="3">
         <v>3.737669618</v>
       </c>
-      <c r="V5" s="5">
+      <c r="V5" s="3">
         <v>6.8354700000000004E-2</v>
       </c>
-      <c r="W5" s="5">
+      <c r="W5" s="3">
         <v>0.83304299999999998</v>
       </c>
-      <c r="X5" s="5">
+      <c r="X5" s="3">
         <v>0.21460658699999999</v>
       </c>
-      <c r="Y5" s="5">
+      <c r="Y5" s="3">
         <v>20.774964300000001</v>
       </c>
-      <c r="Z5" s="5">
+      <c r="Z5" s="3">
         <v>4</v>
       </c>
-      <c r="AA5" s="5">
+      <c r="AA5" s="3">
         <v>44</v>
       </c>
-      <c r="AB5" s="5">
+      <c r="AB5" s="3">
         <v>3.7841896340000001</v>
       </c>
-      <c r="AC5" s="5">
+      <c r="AC5" s="3">
         <v>0.25120100000000001</v>
       </c>
-      <c r="AD5" s="5">
+      <c r="AD5" s="3">
         <v>0.92181716000000002</v>
       </c>
-      <c r="AE5" s="5">
+      <c r="AE5" s="3">
         <v>0.13095680000000001</v>
       </c>
-      <c r="AF5" s="5">
+      <c r="AF5" s="3">
         <v>25.763114999999999</v>
       </c>
-      <c r="AG5" s="5">
+      <c r="AG5" s="3">
         <v>4</v>
       </c>
-      <c r="AH5" s="5">
+      <c r="AH5" s="3">
         <v>26.75</v>
       </c>
-      <c r="AI5" s="5">
+      <c r="AI5" s="3">
         <v>3.2865344730000001</v>
       </c>
-      <c r="AJ5" s="5">
+      <c r="AJ5" s="3">
         <v>0.27088499999999999</v>
       </c>
-      <c r="AK5" s="5">
+      <c r="AK5" s="3">
         <v>0.88848550000000004</v>
       </c>
-      <c r="AL5" s="5">
+      <c r="AL5" s="3">
         <v>0.21741340000000001</v>
       </c>
-      <c r="AM5" s="5">
+      <c r="AM5" s="3">
         <v>14.880421999999999</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>37</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>24</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>14</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>6</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>617</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>339</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="3">
         <v>5</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <v>1139</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="3">
         <v>409</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="3">
         <v>78.918918919999996</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="3">
         <v>4.3680000000000003</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="3">
         <v>0.22577838</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="3">
         <v>0.98815768999999998</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="3">
         <v>0.16004573</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="3">
         <v>37.613250000000001</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S6" s="3">
         <v>10</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6" s="3">
         <v>39.6</v>
       </c>
-      <c r="U6" s="5">
+      <c r="U6" s="3">
         <v>3.6788291179999999</v>
       </c>
-      <c r="V6" s="5">
+      <c r="V6" s="3">
         <v>0.20273479999999999</v>
       </c>
-      <c r="W6" s="5">
+      <c r="W6" s="3">
         <v>0.95153089999999996</v>
       </c>
-      <c r="X6" s="5">
+      <c r="X6" s="3">
         <v>0.21101829999999999</v>
       </c>
-      <c r="Y6" s="5">
+      <c r="Y6" s="3">
         <v>19.305017800000002</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="Z6" s="3">
         <v>13</v>
       </c>
-      <c r="AA6" s="5">
+      <c r="AA6" s="3">
         <v>98.307623000000007</v>
       </c>
-      <c r="AB6" s="5">
+      <c r="AB6" s="3">
         <v>4.5881015720000002</v>
       </c>
-      <c r="AC6" s="5">
+      <c r="AC6" s="3">
         <v>0.1945355</v>
       </c>
-      <c r="AD6" s="5">
+      <c r="AD6" s="3">
         <v>0.97013300000000002</v>
       </c>
-      <c r="AE6" s="5">
+      <c r="AE6" s="3">
         <v>0.14635500000000001</v>
       </c>
-      <c r="AF6" s="5">
+      <c r="AF6" s="3">
         <v>45.153503999999998</v>
       </c>
-      <c r="AG6" s="5">
+      <c r="AG6" s="3">
         <v>14</v>
       </c>
-      <c r="AH6" s="5">
+      <c r="AH6" s="3">
         <v>80.357142859999996</v>
       </c>
-      <c r="AI6" s="5">
+      <c r="AI6" s="3">
         <v>4.3864809850000004</v>
       </c>
-      <c r="AJ6" s="5">
+      <c r="AJ6" s="3">
         <v>0.25814009999999998</v>
       </c>
-      <c r="AK6" s="5">
+      <c r="AK6" s="3">
         <v>0.97317739999999997</v>
       </c>
-      <c r="AL6" s="5">
+      <c r="AL6" s="3">
         <v>0.15760465000000001</v>
       </c>
-      <c r="AM6" s="5">
+      <c r="AM6" s="3">
         <v>41.369053000000001</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="5">
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3">
         <v>15</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>28</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>17</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <v>7</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>1312</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="3">
         <v>838</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="3">
         <v>7</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="3">
         <v>2412</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="3">
         <v>874</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="3">
         <v>79</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="3">
         <v>4.3689999999999998</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="3">
         <v>0.147049867</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="3">
         <v>0.97194899700000004</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="3">
         <v>0.16261800500000001</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="3">
         <v>37.322527700000002</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S7" s="3">
         <v>5</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="3">
         <v>58.6</v>
       </c>
-      <c r="U7" s="5">
+      <c r="U7" s="3">
         <v>4.0707346969999998</v>
       </c>
-      <c r="V7" s="5">
+      <c r="V7" s="3">
         <v>9.0848799999999993E-2</v>
       </c>
-      <c r="W7" s="5">
+      <c r="W7" s="3">
         <v>0.91261479999999995</v>
       </c>
-      <c r="X7" s="5">
+      <c r="X7" s="3">
         <v>0.22462080000000001</v>
       </c>
-      <c r="Y7" s="5">
+      <c r="Y7" s="3">
         <v>31.11627</v>
       </c>
-      <c r="Z7" s="5">
+      <c r="Z7" s="3">
         <v>6</v>
       </c>
-      <c r="AA7" s="5">
+      <c r="AA7" s="3">
         <v>83.833330000000004</v>
       </c>
-      <c r="AB7" s="5">
+      <c r="AB7" s="3">
         <v>4.4288306610000001</v>
       </c>
-      <c r="AC7" s="5">
+      <c r="AC7" s="3">
         <v>0.18026929999999999</v>
       </c>
-      <c r="AD7" s="5">
+      <c r="AD7" s="3">
         <v>0.94726399999999999</v>
       </c>
-      <c r="AE7" s="5">
+      <c r="AE7" s="3">
         <v>0.10780438000000001</v>
       </c>
-      <c r="AF7" s="5">
+      <c r="AF7" s="3">
         <v>38.929560000000002</v>
       </c>
-      <c r="AG7" s="5">
+      <c r="AG7" s="3">
         <v>4</v>
       </c>
-      <c r="AH7" s="5">
+      <c r="AH7" s="3">
         <v>86</v>
       </c>
-      <c r="AI7" s="5">
+      <c r="AI7" s="3">
         <v>4.4543472959999999</v>
       </c>
-      <c r="AJ7" s="5">
+      <c r="AJ7" s="3">
         <v>0.18246100000000001</v>
       </c>
-      <c r="AK7" s="5">
+      <c r="AK7" s="3">
         <v>0.89734499999999995</v>
       </c>
-      <c r="AL7" s="5">
+      <c r="AL7" s="3">
         <v>0.17265739999999999</v>
       </c>
-      <c r="AM7" s="5">
+      <c r="AM7" s="3">
         <v>41.121474999999997</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>9</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>27</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>15</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <v>7</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <v>675</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <v>287</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="3">
         <v>6</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="3">
         <v>1499</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="3">
         <v>439</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="3">
         <v>88.555555560000002</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="3">
         <v>4.484</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="3">
         <v>9.1175779999999998E-2</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="3">
         <v>0.94240409999999997</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8" s="3">
         <v>0.17643013599999999</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="3">
         <v>42.965635599999999</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="3">
         <v>2</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="3">
         <v>58</v>
       </c>
-      <c r="U8" s="5">
+      <c r="U8" s="3">
         <v>4.0604430110000003</v>
       </c>
-      <c r="V8" s="5">
+      <c r="V8" s="3">
         <v>9.4403000000000001E-2</v>
       </c>
-      <c r="W8" s="5">
+      <c r="W8" s="3">
         <v>0.83704849999999997</v>
       </c>
-      <c r="X8" s="5">
+      <c r="X8" s="3">
         <v>0.19617329999999999</v>
       </c>
-      <c r="Y8" s="5">
+      <c r="Y8" s="3">
         <v>28.998619999999999</v>
       </c>
-      <c r="Z8" s="5">
+      <c r="Z8" s="3">
         <v>4</v>
       </c>
-      <c r="AA8" s="5">
+      <c r="AA8" s="3">
         <v>65.75</v>
       </c>
-      <c r="AB8" s="5">
+      <c r="AB8" s="3">
         <v>4.1858596710000002</v>
       </c>
-      <c r="AC8" s="5">
+      <c r="AC8" s="3">
         <v>0.118965</v>
       </c>
-      <c r="AD8" s="5">
+      <c r="AD8" s="3">
         <v>0.91111702000000006</v>
       </c>
-      <c r="AE8" s="5">
+      <c r="AE8" s="3">
         <v>0.16640920000000001</v>
       </c>
-      <c r="AF8" s="5">
+      <c r="AF8" s="3">
         <v>35.049860000000002</v>
       </c>
-      <c r="AG8" s="5">
+      <c r="AG8" s="3">
         <v>3</v>
       </c>
-      <c r="AH8" s="5">
+      <c r="AH8" s="3">
         <v>133.66667000000001</v>
       </c>
-      <c r="AI8" s="5">
+      <c r="AI8" s="3">
         <v>4.8953491639999998</v>
       </c>
-      <c r="AJ8" s="5">
+      <c r="AJ8" s="3">
         <v>4.8706670000000001E-2</v>
       </c>
-      <c r="AK8" s="5">
+      <c r="AK8" s="3">
         <v>0.8599755</v>
       </c>
-      <c r="AL8" s="5">
+      <c r="AL8" s="3">
         <v>0.18090389700000001</v>
       </c>
-      <c r="AM8" s="5">
+      <c r="AM8" s="3">
         <v>60.215957000000003</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="3">
         <v>25</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>1</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>23</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>16</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="3">
         <v>8</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <v>968</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="3">
         <v>549</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="3">
         <v>6</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="3">
         <v>2014</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="3">
         <v>784</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="3">
         <v>69.12</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="3">
         <v>4.2359999999999998</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="3">
         <v>0.30596751999999999</v>
       </c>
-      <c r="P9" s="5">
+      <c r="P9" s="3">
         <v>0.98199672299999996</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="Q9" s="3">
         <v>0.131104952</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="3">
         <v>35.525865060000001</v>
       </c>
-      <c r="S9" s="5">
+      <c r="S9" s="3">
         <v>7</v>
       </c>
-      <c r="T9" s="5">
+      <c r="T9" s="3">
         <v>90.857142999999994</v>
       </c>
-      <c r="U9" s="5">
+      <c r="U9" s="3">
         <v>4.5092884160000004</v>
       </c>
-      <c r="V9" s="5">
+      <c r="V9" s="3">
         <v>0.18108940000000001</v>
       </c>
-      <c r="W9" s="5">
+      <c r="W9" s="3">
         <v>0.94469440000000005</v>
       </c>
-      <c r="X9" s="5">
+      <c r="X9" s="3">
         <v>0.1624439</v>
       </c>
-      <c r="Y9" s="5">
+      <c r="Y9" s="3">
         <v>44.379280000000001</v>
       </c>
-      <c r="Z9" s="5">
+      <c r="Z9" s="3">
         <v>11</v>
       </c>
-      <c r="AA9" s="5">
+      <c r="AA9" s="3">
         <v>68.363630000000001</v>
       </c>
-      <c r="AB9" s="5">
+      <c r="AB9" s="3">
         <v>4.2248409579999997</v>
       </c>
-      <c r="AC9" s="5">
+      <c r="AC9" s="3">
         <v>0.2334736</v>
       </c>
-      <c r="AD9" s="5">
+      <c r="AD9" s="3">
         <v>0.96119986000000002</v>
       </c>
-      <c r="AE9" s="5">
+      <c r="AE9" s="3">
         <v>0.13990900000000001</v>
       </c>
-      <c r="AF9" s="5">
+      <c r="AF9" s="3">
         <v>36.888300000000001</v>
       </c>
-      <c r="AG9" s="5">
+      <c r="AG9" s="3">
         <v>7</v>
       </c>
-      <c r="AH9" s="5">
+      <c r="AH9" s="3">
         <v>50.285710000000002</v>
       </c>
-      <c r="AI9" s="5">
+      <c r="AI9" s="3">
         <v>3.9177209409999998</v>
       </c>
-      <c r="AJ9" s="5">
+      <c r="AJ9" s="3">
         <v>0.53648399999999996</v>
       </c>
-      <c r="AK9" s="5">
+      <c r="AK9" s="3">
         <v>0.95042899999999997</v>
       </c>
-      <c r="AL9" s="5">
+      <c r="AL9" s="3">
         <v>0.10155930000000001</v>
       </c>
-      <c r="AM9" s="5">
+      <c r="AM9" s="3">
         <v>28.399778000000001</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>23</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>1</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>19</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>15</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="3">
         <v>3</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="3">
         <v>585</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="3">
         <v>373</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="3">
         <v>1</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="3">
         <v>1162</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="3">
         <v>561</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="3">
         <v>193.69565220000001</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="3">
         <v>5.266</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="3">
         <v>9.5478869999999993E-2</v>
       </c>
-      <c r="P10" s="5">
+      <c r="P10" s="3">
         <v>0.97507823900000001</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="Q10" s="3">
         <v>0.17835653800000001</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10" s="3">
         <v>78.967522650000006</v>
       </c>
-      <c r="S10" s="5">
+      <c r="S10" s="3">
         <v>9</v>
       </c>
-      <c r="T10" s="5">
+      <c r="T10" s="3">
         <v>75.111099999999993</v>
       </c>
-      <c r="U10" s="5">
+      <c r="U10" s="3">
         <v>4.3189683509999997</v>
       </c>
-      <c r="V10" s="5">
+      <c r="V10" s="3">
         <v>0.132576</v>
       </c>
-      <c r="W10" s="5">
+      <c r="W10" s="3">
         <v>0.95246920000000002</v>
       </c>
-      <c r="X10" s="5">
+      <c r="X10" s="3">
         <v>0.21362829999999999</v>
       </c>
-      <c r="Y10" s="5">
+      <c r="Y10" s="3">
         <v>40.348385</v>
       </c>
-      <c r="Z10" s="5">
+      <c r="Z10" s="3">
         <v>6</v>
       </c>
-      <c r="AA10" s="5">
+      <c r="AA10" s="3">
         <v>269</v>
       </c>
-      <c r="AB10" s="5">
+      <c r="AB10" s="3">
         <v>5.5947113799999997</v>
       </c>
-      <c r="AC10" s="5">
+      <c r="AC10" s="3">
         <v>4.2849669999999999E-2</v>
       </c>
-      <c r="AD10" s="5">
+      <c r="AD10" s="3">
         <v>0.90994889999999995</v>
       </c>
-      <c r="AE10" s="5">
+      <c r="AE10" s="3">
         <v>0.19885459999999999</v>
       </c>
-      <c r="AF10" s="5">
+      <c r="AF10" s="3">
         <v>103.0326</v>
       </c>
-      <c r="AG10" s="5">
+      <c r="AG10" s="3">
         <v>8</v>
       </c>
-      <c r="AH10" s="5">
+      <c r="AH10" s="3">
         <v>259.375</v>
       </c>
-      <c r="AI10" s="5">
+      <c r="AI10" s="3">
         <v>5.5582748909999999</v>
       </c>
-      <c r="AJ10" s="5">
+      <c r="AJ10" s="3">
         <v>8.9593999999999993E-2</v>
       </c>
-      <c r="AK10" s="5">
+      <c r="AK10" s="3">
         <v>0.93827970000000005</v>
       </c>
-      <c r="AL10" s="5">
+      <c r="AL10" s="3">
         <v>0.13887679999999999</v>
       </c>
-      <c r="AM10" s="5">
+      <c r="AM10" s="3">
         <v>100.56278</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>2</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>1</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>36</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>24</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="3">
         <v>14</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="3">
         <v>1010</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="3">
         <v>454</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="3">
         <v>8</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="3">
         <v>2218</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="3">
         <v>641</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="3">
         <v>55.5</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="3">
         <v>4.016</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="3">
         <v>0.15984000000000001</v>
       </c>
-      <c r="P11" s="5">
+      <c r="P11" s="3">
         <v>0.86271717199999998</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="Q11" s="3">
         <v>0.137399991</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="3">
         <v>28.305678</v>
       </c>
-      <c r="S11" s="5">
+      <c r="S11" s="3">
         <v>1</v>
       </c>
-      <c r="T11" s="5">
+      <c r="T11" s="3">
         <v>44</v>
       </c>
-      <c r="U11" s="5">
+      <c r="U11" s="3">
         <v>3.7841896340000001</v>
       </c>
-      <c r="V11" s="5">
+      <c r="V11" s="3">
         <v>3.0575000000000001E-2</v>
       </c>
-      <c r="W11" s="5">
+      <c r="W11" s="3">
         <v>0.8246945</v>
       </c>
-      <c r="X11" s="5">
+      <c r="X11" s="3">
         <v>0.2069484</v>
       </c>
-      <c r="Y11" s="5">
+      <c r="Y11" s="3">
         <v>17.204049999999999</v>
       </c>
-      <c r="Z11" s="5">
+      <c r="Z11" s="3">
         <v>1</v>
       </c>
-      <c r="AA11" s="5">
+      <c r="AA11" s="3">
         <v>62</v>
       </c>
-      <c r="AB11" s="5">
+      <c r="AB11" s="3">
         <v>4.1271343849999997</v>
       </c>
-      <c r="AC11" s="5">
+      <c r="AC11" s="3">
         <v>0.219392</v>
       </c>
-      <c r="AD11" s="5">
+      <c r="AD11" s="3">
         <v>0.78387099999999998</v>
       </c>
-      <c r="AE11" s="5">
+      <c r="AE11" s="3">
         <v>7.3516956999999994E-2</v>
       </c>
-      <c r="AF11" s="5">
+      <c r="AF11" s="3">
         <v>40.472279999999998</v>
       </c>
-      <c r="AG11" s="5">
+      <c r="AG11" s="3">
         <v>3</v>
       </c>
-      <c r="AH11" s="5">
+      <c r="AH11" s="3">
         <v>64.332999999999998</v>
       </c>
-      <c r="AI11" s="5">
+      <c r="AI11" s="3">
         <v>4.164072719</v>
       </c>
-      <c r="AJ11" s="5">
+      <c r="AJ11" s="3">
         <v>0.58982467000000005</v>
       </c>
-      <c r="AK11" s="5">
+      <c r="AK11" s="3">
         <v>0.94734496000000001</v>
       </c>
-      <c r="AL11" s="5">
+      <c r="AL11" s="3">
         <v>3.1665800000000001E-2</v>
       </c>
-      <c r="AM11" s="5">
+      <c r="AM11" s="3">
         <v>37.734589999999997</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>3</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>32</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>17</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="3">
         <v>7</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="3">
         <v>959</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="3">
         <v>536</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="3">
         <v>8</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="3">
         <v>2062</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="3">
         <v>749</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="3">
         <v>73.666669999999996</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="3">
         <v>4.3</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="3">
         <v>0.33417732999999999</v>
       </c>
-      <c r="P12" s="5">
+      <c r="P12" s="3">
         <v>0.873</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="3">
         <v>0.13885510000000001</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12" s="3">
         <v>43.619243500000003</v>
       </c>
-      <c r="S12" s="5">
+      <c r="S12" s="3">
         <v>1</v>
       </c>
-      <c r="T12" s="5">
+      <c r="T12" s="3">
         <v>73</v>
       </c>
-      <c r="U12" s="5">
+      <c r="U12" s="3">
         <v>4.2904594410000003</v>
       </c>
-      <c r="V12" s="5">
+      <c r="V12" s="3">
         <v>7.6034000000000004E-2</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W12" s="3">
         <v>0.7070959</v>
       </c>
-      <c r="X12" s="5">
+      <c r="X12" s="3">
         <v>0.18016450000000001</v>
       </c>
-      <c r="Y12" s="5">
+      <c r="Y12" s="3">
         <v>38.646819999999998</v>
       </c>
-      <c r="Z12" s="5">
+      <c r="Z12" s="3">
         <v>1</v>
       </c>
-      <c r="AA12" s="5">
+      <c r="AA12" s="3">
         <v>42</v>
       </c>
-      <c r="AB12" s="5">
+      <c r="AB12" s="3">
         <v>3.737669618</v>
       </c>
-      <c r="AC12" s="5">
+      <c r="AC12" s="3">
         <v>0.25883</v>
       </c>
-      <c r="AD12" s="5">
+      <c r="AD12" s="3">
         <v>0.81304759999999998</v>
       </c>
-      <c r="AE12" s="5">
+      <c r="AE12" s="3">
         <v>9.1989000000000001E-2</v>
       </c>
-      <c r="AF12" s="5">
+      <c r="AF12" s="3">
         <v>27.123239999999999</v>
       </c>
-      <c r="AG12" s="5">
+      <c r="AG12" s="3">
         <v>1</v>
       </c>
-      <c r="AH12" s="5">
+      <c r="AH12" s="3">
         <v>86</v>
       </c>
-      <c r="AI12" s="5">
+      <c r="AI12" s="3">
         <v>4.4543472959999999</v>
       </c>
-      <c r="AJ12" s="5">
+      <c r="AJ12" s="3">
         <v>7.2095999999999993E-2</v>
       </c>
-      <c r="AK12" s="5">
+      <c r="AK12" s="3">
         <v>0.71739529999999996</v>
       </c>
-      <c r="AL12" s="5">
+      <c r="AL12" s="3">
         <v>0.16128366</v>
       </c>
-      <c r="AM12" s="5">
+      <c r="AM12" s="3">
         <v>45.698669000000002</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="A13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3">
         <v>6</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <v>1</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>27</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
         <v>18</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="3">
         <v>5</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="3">
         <v>849</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="3">
         <v>612</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="3">
         <v>1</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="3">
         <v>1357</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="3">
         <v>747</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="3">
         <v>56.5</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="3">
         <v>4.0339999999999998</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="3">
         <v>0.224815667</v>
       </c>
-      <c r="P13" s="5">
+      <c r="P13" s="3">
         <v>0.95031019999999999</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="Q13" s="3">
         <v>0.15887883</v>
       </c>
-      <c r="R13" s="5">
+      <c r="R13" s="3">
         <v>30.415714999999999</v>
       </c>
-      <c r="S13" s="5">
+      <c r="S13" s="3">
         <v>3</v>
       </c>
-      <c r="T13" s="5">
+      <c r="T13" s="3">
         <v>48.333300000000001</v>
       </c>
-      <c r="U13" s="5">
+      <c r="U13" s="3">
         <v>3.8781207640000002</v>
       </c>
-      <c r="V13" s="5">
+      <c r="V13" s="3">
         <v>0.13121267</v>
       </c>
-      <c r="W13" s="5">
+      <c r="W13" s="3">
         <v>0.87948999999999999</v>
       </c>
-      <c r="X13" s="5">
+      <c r="X13" s="3">
         <v>0.20073199999999999</v>
       </c>
-      <c r="Y13" s="5">
+      <c r="Y13" s="3">
         <v>27.799430000000001</v>
       </c>
-      <c r="Z13" s="5">
+      <c r="Z13" s="3">
         <v>2</v>
       </c>
-      <c r="AA13" s="5">
+      <c r="AA13" s="3">
         <v>83</v>
       </c>
-      <c r="AB13" s="5">
+      <c r="AB13" s="3">
         <v>4.418840608</v>
       </c>
-      <c r="AC13" s="5">
+      <c r="AC13" s="3">
         <v>0.402949</v>
       </c>
-      <c r="AD13" s="5">
+      <c r="AD13" s="3">
         <v>0.90616350000000001</v>
       </c>
-      <c r="AE13" s="5">
+      <c r="AE13" s="3">
         <v>5.5979769999999998E-2</v>
       </c>
-      <c r="AF13" s="5">
+      <c r="AF13" s="3">
         <v>41.48227</v>
       </c>
-      <c r="AG13" s="5">
+      <c r="AG13" s="3">
         <v>1</v>
       </c>
-      <c r="AH13" s="5">
+      <c r="AH13" s="3">
         <v>28</v>
       </c>
-      <c r="AI13" s="5">
+      <c r="AI13" s="3">
         <v>3.33220451</v>
       </c>
-      <c r="AJ13" s="5">
+      <c r="AJ13" s="3">
         <v>0.14935799999999999</v>
       </c>
-      <c r="AK13" s="5">
+      <c r="AK13" s="3">
         <v>0.6847143</v>
       </c>
-      <c r="AL13" s="5">
+      <c r="AL13" s="3">
         <v>0.23911867000000001</v>
       </c>
-      <c r="AM13" s="5">
+      <c r="AM13" s="3">
         <v>16.131439</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="A14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="3">
         <v>15</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="3">
         <v>29</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="3">
         <v>21</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="3">
         <v>6</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="3">
         <v>817</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="3">
         <v>519</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="3">
         <v>2</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="3">
         <v>1545</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="3">
         <v>764</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="3">
         <v>114.266667</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="3">
         <v>4.7389999999999999</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="3">
         <v>0.29667830000000001</v>
       </c>
-      <c r="P14" s="5">
+      <c r="P14" s="3">
         <v>0.97210111700000001</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="Q14" s="3">
         <v>0.17197025499999999</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="3">
         <v>40.941246100000001</v>
       </c>
-      <c r="S14" s="5">
+      <c r="S14" s="3">
         <v>5</v>
       </c>
-      <c r="T14" s="5">
+      <c r="T14" s="3">
         <v>74.400000000000006</v>
       </c>
-      <c r="U14" s="5">
+      <c r="U14" s="3">
         <v>4.3094559419999996</v>
       </c>
-      <c r="V14" s="5">
+      <c r="V14" s="3">
         <v>0.367732</v>
       </c>
-      <c r="W14" s="5">
+      <c r="W14" s="3">
         <v>0.92711209999999999</v>
       </c>
-      <c r="X14" s="5">
+      <c r="X14" s="3">
         <v>0.15188280000000001</v>
       </c>
-      <c r="Y14" s="5">
+      <c r="Y14" s="3">
         <v>36.250360000000001</v>
       </c>
-      <c r="Z14" s="5">
+      <c r="Z14" s="3">
         <v>5</v>
       </c>
-      <c r="AA14" s="5">
+      <c r="AA14" s="3">
         <v>183.4</v>
       </c>
-      <c r="AB14" s="5">
+      <c r="AB14" s="3">
         <v>5.2116695599999998</v>
       </c>
-      <c r="AC14" s="5">
+      <c r="AC14" s="3">
         <v>4.7849999999999997E-2</v>
       </c>
-      <c r="AD14" s="5">
+      <c r="AD14" s="3">
         <v>0.9214002</v>
       </c>
-      <c r="AE14" s="5">
+      <c r="AE14" s="3">
         <v>0.17617099999999999</v>
       </c>
-      <c r="AF14" s="5">
+      <c r="AF14" s="3">
         <v>76.909530000000004</v>
       </c>
-      <c r="AG14" s="5">
+      <c r="AG14" s="3">
         <v>5</v>
       </c>
-      <c r="AH14" s="5">
+      <c r="AH14" s="3">
         <v>85</v>
       </c>
-      <c r="AI14" s="5">
+      <c r="AI14" s="3">
         <v>4.4426512560000004</v>
       </c>
-      <c r="AJ14" s="5">
+      <c r="AJ14" s="3">
         <v>0.47445300000000001</v>
       </c>
-      <c r="AK14" s="5">
+      <c r="AK14" s="3">
         <v>0.92191440000000002</v>
       </c>
-      <c r="AL14" s="5">
+      <c r="AL14" s="3">
         <v>0.187857</v>
       </c>
-      <c r="AM14" s="5">
+      <c r="AM14" s="3">
         <v>36.663849999999996</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>